<commit_message>
removed Flags column and calculated new Index_DE
</commit_message>
<xml_diff>
--- a/all_DE/Benedikt XVI.xlsx
+++ b/all_DE/Benedikt XVI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phildickson/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johanna\Documents\GitHub\COINS_SwissTribeleaders\all_DE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2125FFFA-E56E-1C42-A60A-6907B9A9A401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F401CB3-1403-4F1B-A428-23644FD048F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{DEE577B7-EB13-40D6-A095-037F5B5CCD1E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DEE577B7-EB13-40D6-A095-037F5B5CCD1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="443">
   <si>
     <t>title</t>
   </si>
@@ -1717,9 +1717,6 @@
 Aber warum hat es so lange gedauert, bis ein Papst eine Moschee besucht hat?
 Vor dem Besuch 2001 hat er schon viele Muslime getroffen.
 DOMRADIO.DE: Das war wirklich ein beeindruckendes Bild damals, wie der Papst und der syrische Großmufti zusammen die Moschee betreten haben.</t>
-  </si>
-  <si>
-    <t>flag</t>
   </si>
 </sst>
 </file>
@@ -1762,7 +1759,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1785,32 +1782,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -2126,15 +2109,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B58983-D882-4CC0-A46B-B2E70AA74484}">
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="K95" sqref="K95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2159,11 +2142,8 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2188,11 +2168,8 @@
       <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2217,11 +2194,8 @@
       <c r="I3" t="s">
         <v>20</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2246,11 +2220,8 @@
       <c r="I4" t="s">
         <v>25</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2275,11 +2246,8 @@
       <c r="I5" t="s">
         <v>30</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2304,11 +2272,8 @@
       <c r="I6" t="s">
         <v>36</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2333,11 +2298,8 @@
       <c r="I7" t="s">
         <v>42</v>
       </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2362,11 +2324,8 @@
       <c r="I8" t="s">
         <v>48</v>
       </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2391,11 +2350,8 @@
       <c r="I9" t="s">
         <v>53</v>
       </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2420,11 +2376,8 @@
       <c r="I10" t="s">
         <v>58</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2449,11 +2402,8 @@
       <c r="I11" t="s">
         <v>64</v>
       </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2478,11 +2428,8 @@
       <c r="I12" t="s">
         <v>69</v>
       </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2507,11 +2454,8 @@
       <c r="I13" t="s">
         <v>73</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2536,11 +2480,8 @@
       <c r="I14" t="s">
         <v>77</v>
       </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2565,11 +2506,8 @@
       <c r="I15" t="s">
         <v>82</v>
       </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2594,11 +2532,8 @@
       <c r="I16" t="s">
         <v>87</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2623,11 +2558,8 @@
       <c r="I17" t="s">
         <v>91</v>
       </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2655,11 +2587,8 @@
       <c r="I18" t="s">
         <v>96</v>
       </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2684,11 +2613,8 @@
       <c r="I19" t="s">
         <v>101</v>
       </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2713,11 +2639,8 @@
       <c r="I20" t="s">
         <v>106</v>
       </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2742,11 +2665,8 @@
       <c r="I21" t="s">
         <v>111</v>
       </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2771,11 +2691,8 @@
       <c r="I22" t="s">
         <v>116</v>
       </c>
-      <c r="J22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2800,11 +2717,8 @@
       <c r="I23" t="s">
         <v>121</v>
       </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2829,11 +2743,8 @@
       <c r="I24" t="s">
         <v>126</v>
       </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2858,11 +2769,8 @@
       <c r="I25" t="s">
         <v>131</v>
       </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2887,11 +2795,8 @@
       <c r="I26" t="s">
         <v>136</v>
       </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2916,11 +2821,8 @@
       <c r="I27" t="s">
         <v>141</v>
       </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2945,11 +2847,8 @@
       <c r="I28" t="s">
         <v>145</v>
       </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2971,11 +2870,8 @@
       <c r="I29" t="s">
         <v>150</v>
       </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -3000,11 +2896,8 @@
       <c r="I30" t="s">
         <v>154</v>
       </c>
-      <c r="J30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3029,11 +2922,8 @@
       <c r="I31" t="s">
         <v>159</v>
       </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3058,11 +2948,8 @@
       <c r="I32" t="s">
         <v>165</v>
       </c>
-      <c r="J32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3087,11 +2974,8 @@
       <c r="I33" t="s">
         <v>170</v>
       </c>
-      <c r="J33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3116,11 +3000,8 @@
       <c r="I34" t="s">
         <v>175</v>
       </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3145,11 +3026,8 @@
       <c r="I35" t="s">
         <v>181</v>
       </c>
-      <c r="J35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3174,11 +3052,8 @@
       <c r="I36" t="s">
         <v>186</v>
       </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3203,11 +3078,8 @@
       <c r="I37" t="s">
         <v>191</v>
       </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3232,11 +3104,8 @@
       <c r="I38" t="s">
         <v>195</v>
       </c>
-      <c r="J38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3261,11 +3130,8 @@
       <c r="I39" t="s">
         <v>200</v>
       </c>
-      <c r="J39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3290,11 +3156,8 @@
       <c r="I40" t="s">
         <v>206</v>
       </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3319,11 +3182,8 @@
       <c r="I41" t="s">
         <v>210</v>
       </c>
-      <c r="J41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3348,11 +3208,8 @@
       <c r="I42" t="s">
         <v>216</v>
       </c>
-      <c r="J42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3377,11 +3234,8 @@
       <c r="I43" t="s">
         <v>220</v>
       </c>
-      <c r="J43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3406,11 +3260,8 @@
       <c r="I44" t="s">
         <v>224</v>
       </c>
-      <c r="J44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -3435,11 +3286,8 @@
       <c r="I45" t="s">
         <v>229</v>
       </c>
-      <c r="J45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -3464,11 +3312,8 @@
       <c r="I46" t="s">
         <v>233</v>
       </c>
-      <c r="J46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3493,11 +3338,8 @@
       <c r="I47" t="s">
         <v>238</v>
       </c>
-      <c r="J47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3522,11 +3364,8 @@
       <c r="I48" t="s">
         <v>242</v>
       </c>
-      <c r="J48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3551,11 +3390,8 @@
       <c r="I49" t="s">
         <v>247</v>
       </c>
-      <c r="J49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3580,11 +3416,8 @@
       <c r="I50" t="s">
         <v>252</v>
       </c>
-      <c r="J50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3609,11 +3442,8 @@
       <c r="I51" t="s">
         <v>257</v>
       </c>
-      <c r="J51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3638,11 +3468,8 @@
       <c r="I52" t="s">
         <v>262</v>
       </c>
-      <c r="J52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3667,11 +3494,8 @@
       <c r="I53" t="s">
         <v>267</v>
       </c>
-      <c r="J53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3696,11 +3520,8 @@
       <c r="I54" t="s">
         <v>271</v>
       </c>
-      <c r="J54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3725,11 +3546,8 @@
       <c r="I55" t="s">
         <v>276</v>
       </c>
-      <c r="J55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3754,11 +3572,8 @@
       <c r="I56" t="s">
         <v>281</v>
       </c>
-      <c r="J56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -3783,11 +3598,8 @@
       <c r="I57" t="s">
         <v>285</v>
       </c>
-      <c r="J57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -3812,11 +3624,8 @@
       <c r="I58" t="s">
         <v>290</v>
       </c>
-      <c r="J58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3841,11 +3650,8 @@
       <c r="I59" t="s">
         <v>295</v>
       </c>
-      <c r="J59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3870,11 +3676,8 @@
       <c r="I60" t="s">
         <v>300</v>
       </c>
-      <c r="J60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3899,11 +3702,8 @@
       <c r="I61" t="s">
         <v>304</v>
       </c>
-      <c r="J61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3928,11 +3728,8 @@
       <c r="I62" t="s">
         <v>309</v>
       </c>
-      <c r="J62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -3957,11 +3754,8 @@
       <c r="I63" t="s">
         <v>313</v>
       </c>
-      <c r="J63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -3986,11 +3780,8 @@
       <c r="I64" t="s">
         <v>318</v>
       </c>
-      <c r="J64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -4015,11 +3806,8 @@
       <c r="I65" t="s">
         <v>322</v>
       </c>
-      <c r="J65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -4044,11 +3832,8 @@
       <c r="I66" t="s">
         <v>327</v>
       </c>
-      <c r="J66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -4073,11 +3858,8 @@
       <c r="I67" t="s">
         <v>332</v>
       </c>
-      <c r="J67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -4102,11 +3884,8 @@
       <c r="I68" t="s">
         <v>338</v>
       </c>
-      <c r="J68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -4131,11 +3910,8 @@
       <c r="I69" t="s">
         <v>344</v>
       </c>
-      <c r="J69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -4160,11 +3936,8 @@
       <c r="I70" t="s">
         <v>349</v>
       </c>
-      <c r="J70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -4189,11 +3962,8 @@
       <c r="I71" t="s">
         <v>353</v>
       </c>
-      <c r="J71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -4218,11 +3988,8 @@
       <c r="I72" t="s">
         <v>358</v>
       </c>
-      <c r="J72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -4247,11 +4014,8 @@
       <c r="I73" t="s">
         <v>363</v>
       </c>
-      <c r="J73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -4276,11 +4040,8 @@
       <c r="I74" t="s">
         <v>368</v>
       </c>
-      <c r="J74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -4305,11 +4066,8 @@
       <c r="I75" t="s">
         <v>372</v>
       </c>
-      <c r="J75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -4334,11 +4092,8 @@
       <c r="I76" t="s">
         <v>376</v>
       </c>
-      <c r="J76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -4363,11 +4118,8 @@
       <c r="I77" t="s">
         <v>382</v>
       </c>
-      <c r="J77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -4392,11 +4144,8 @@
       <c r="I78" t="s">
         <v>387</v>
       </c>
-      <c r="J78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -4421,11 +4170,8 @@
       <c r="I79" t="s">
         <v>392</v>
       </c>
-      <c r="J79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -4450,11 +4196,8 @@
       <c r="I80" t="s">
         <v>397</v>
       </c>
-      <c r="J80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -4479,11 +4222,8 @@
       <c r="I81" t="s">
         <v>402</v>
       </c>
-      <c r="J81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -4511,11 +4251,8 @@
       <c r="I82" t="s">
         <v>406</v>
       </c>
-      <c r="J82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -4543,11 +4280,8 @@
       <c r="I83" t="s">
         <v>409</v>
       </c>
-      <c r="J83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -4575,11 +4309,8 @@
       <c r="I84" t="s">
         <v>413</v>
       </c>
-      <c r="J84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -4604,11 +4335,8 @@
       <c r="I85" t="s">
         <v>417</v>
       </c>
-      <c r="J85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -4636,11 +4364,8 @@
       <c r="I86" t="s">
         <v>421</v>
       </c>
-      <c r="J86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -4668,11 +4393,8 @@
       <c r="I87" t="s">
         <v>426</v>
       </c>
-      <c r="J87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -4700,11 +4422,8 @@
       <c r="I88" t="s">
         <v>430</v>
       </c>
-      <c r="J88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -4732,11 +4451,8 @@
       <c r="I89" t="s">
         <v>434</v>
       </c>
-      <c r="J89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -4764,11 +4480,8 @@
       <c r="I90" t="s">
         <v>438</v>
       </c>
-      <c r="J90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -4795,9 +4508,6 @@
       </c>
       <c r="I91" t="s">
         <v>442</v>
-      </c>
-      <c r="J91">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>